<commit_message>
Final analysis and adjusted metadata (removing dublicate comparison titles)
</commit_message>
<xml_diff>
--- a/metadata/21_GSE145988.xlsx
+++ b/metadata/21_GSE145988.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shdam/Dropbox/05_1_individual_study_excel_KVS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/sohdam_dtu_dk/Documents/Rprojects/pairedGSEA/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D3E98A-5EC0-E749-9178-BBED08D12815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{21D3E98A-5EC0-E749-9178-BBED08D12815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEB4557B-9299-CD43-86DD-2DAB51C4E9FC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>study</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>IMPDH1 knockdown</t>
+  </si>
+  <si>
+    <t>IMPDH2 knockdown</t>
   </si>
 </sst>
 </file>
@@ -150,7 +153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -553,7 +556,7 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>